<commit_message>
Hello from the other side :)
</commit_message>
<xml_diff>
--- a/WIP/files/Q14.xlsx
+++ b/WIP/files/Q14.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA5341D-FB88-4C1C-BE23-A3693D9C04DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAD0DA-1DC7-421F-91B9-E23E68A6242F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -1777,7 +1777,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C03733B-F283-4EBC-A293-E57D0B4FFCA2}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2454,6 +2454,28 @@
         <v>140</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>